<commit_message>
Add First Files to ETL
</commit_message>
<xml_diff>
--- a/data/files/Initial_data.xlsx
+++ b/data/files/Initial_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galigaribaldi/go/src/github.com/galigaribaldi/PersonalBooks/data/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E186EC1B-10B6-304E-9218-0C48331142E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E72E74B-DA28-8743-BD35-04366055ED15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{94D4D9AC-B6ED-1544-875A-9F2EA1745E3B}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15980" activeTab="1" xr2:uid="{94D4D9AC-B6ED-1544-875A-9F2EA1745E3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="CommentAuthor" sheetId="4" r:id="rId4"/>
     <sheet name="Calification" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,12 +38,399 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="122">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>AUTHOR</t>
+  </si>
+  <si>
+    <t>EDITORIAL</t>
+  </si>
+  <si>
+    <t>SAGA</t>
+  </si>
+  <si>
+    <t>NUMERO_PAGINAS</t>
+  </si>
+  <si>
+    <t>ANIO_PUBLICACION</t>
+  </si>
+  <si>
+    <t>LINK_PORTADA</t>
+  </si>
+  <si>
+    <t>SINOPSIS</t>
+  </si>
+  <si>
+    <t>Flores en el Ático</t>
+  </si>
+  <si>
+    <t>Caballo de Troya</t>
+  </si>
+  <si>
+    <t>El complot Mongol</t>
+  </si>
+  <si>
+    <t>El guardían entre el centeno</t>
+  </si>
+  <si>
+    <t>La Campana de Cristal</t>
+  </si>
+  <si>
+    <t>Si decido Quedarme</t>
+  </si>
+  <si>
+    <t>Harry Potter y El Cáliz de Fuego</t>
+  </si>
+  <si>
+    <t>Harry Potter y La Piedra Filosofal</t>
+  </si>
+  <si>
+    <t>Harry Potter y La Cámara Secreta</t>
+  </si>
+  <si>
+    <t>Harry Potter y El Prisionero de Azkaban</t>
+  </si>
+  <si>
+    <t>Harry Potter y la Órden del Fenix</t>
+  </si>
+  <si>
+    <t>El hombre en el Castillo</t>
+  </si>
+  <si>
+    <t>México Bárbaro</t>
+  </si>
+  <si>
+    <t>El Llano en Llamas</t>
+  </si>
+  <si>
+    <t>It (Eso)</t>
+  </si>
+  <si>
+    <t>El Resplandor</t>
+  </si>
+  <si>
+    <t>Sherlock Holmes, Estudio en Escarlata</t>
+  </si>
+  <si>
+    <t>Sherlock Holmes, El signo de los 4</t>
+  </si>
+  <si>
+    <t>Sherlock Holmes, El sabueso de los Baskerville</t>
+  </si>
+  <si>
+    <t>Persépolis</t>
+  </si>
+  <si>
+    <t>Virginia Cleo Andrews (V.C Andrews)</t>
+  </si>
+  <si>
+    <t>Juan José Benitez (J.J Benitez)</t>
+  </si>
+  <si>
+    <t>Jerome David Salinger (J.D Salinger)</t>
+  </si>
+  <si>
+    <t>Gayle Forman</t>
+  </si>
+  <si>
+    <t>John Kenneth Turner (J.K Turner)</t>
+  </si>
+  <si>
+    <t>Arthur Conan Doyle</t>
+  </si>
+  <si>
+    <t>Marjene Satrappi</t>
+  </si>
+  <si>
+    <t>Dollanganger</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>If I Stay Saga</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>Sherlock Holmes</t>
+  </si>
+  <si>
+    <t>NORMA</t>
+  </si>
+  <si>
+    <t>Planeta</t>
+  </si>
+  <si>
+    <t>Alianza</t>
+  </si>
+  <si>
+    <t>Heinemann</t>
+  </si>
+  <si>
+    <t>Jerusalén, Caballo de Troya</t>
+  </si>
+  <si>
+    <t>DEBOLS!LLO</t>
+  </si>
+  <si>
+    <t>SALAMANDRA INFANTIL Y JUVENIL</t>
+  </si>
+  <si>
+    <t>Pottermore Publishing</t>
+  </si>
+  <si>
+    <t>Philip Kindred Dick (Phillip K. Dick)</t>
+  </si>
+  <si>
+    <t>Ward Lock &amp; Co</t>
+  </si>
+  <si>
+    <t>Minotauro</t>
+  </si>
+  <si>
+    <t>Fondo de Cultura Económica</t>
+  </si>
+  <si>
+    <t>https://www.elsotano.com/imagenes_grandes/9786071/978607141152.JPG</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/81ffybroivL.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/812wOSLnW1L.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/81iniAfNnxL.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/sherlockholmes/images/9/9e/El_sabueso_de_los_Baskerville.jpg/revision/latest/top-crop/width/360/height/450?cb=20140115210200&amp;path-prefix=es</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/51seGWW-wrL.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/81ySgYEwArL.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71NaD6ZH4ZL.jpg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTjovtzDU13lFRv78s4YG3ipvETnKDgYKdp2w&amp;usqp=CAU</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/515J1emcbkL.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/41zqI6oPb-L.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/41q-WZgFyBL.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/51Y6Exe5UiL.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71CZwNUTfpL.jpg</t>
+  </si>
+  <si>
+    <t>https://www.penguinlibros.com/cl/89829/flores-en-el-atico-saga-dollanganger-1.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/61v91uQlNNL.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/91MSyPRab0L.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/81lqVJlb1rL.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71-QfDZfKQL.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71n2N7TJu9L.jpg</t>
+  </si>
+  <si>
+    <t>ANIO_NACIMIENTO</t>
+  </si>
+  <si>
+    <t>ANIO_DEFUNCION</t>
+  </si>
+  <si>
+    <t>PAIS_ORIGEN</t>
+  </si>
+  <si>
+    <t>MOTIVO_DEFUNCION</t>
+  </si>
+  <si>
+    <t>PHOTO_IMG</t>
+  </si>
+  <si>
+    <t>MINI BIOGRAFIA</t>
+  </si>
+  <si>
+    <t>EUA</t>
+  </si>
+  <si>
+    <t>Cáncer de mama</t>
+  </si>
+  <si>
+    <t>Virginia Cleo Andrews, más conocida como V.C. Andrews o Virginia C. Andrews (Portsmouth, Virginia, 6 de junio de 19231​ - Virginia Beach, Virginia, 19 de diciembre de 1986) fue una escritora estadounidense famosa por su novela Flores en el ático.
+Cuando era una adolescente sufrió una caída que le produjo lesiones que la obligaron a permanecer el resto de su vida en una silla de ruedas. Trabajó como artista comercial mientras publicaba varias novelas cortas y relatos en diferentes revistas hasta que su obra Flores en el ático consiguió el número 1 de las listas y se convirtió en una escritora de éxito. Murió a la edad de 63 años de cáncer de mama.</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/2/2f/V._C._Andrews.jpg</t>
+  </si>
+  <si>
+    <t>Juan José Benítez López (Pamplona, 7 de septiembre de 1946),1​ más conocido como J. J. Benítez, es un periodista y escritor español, conocido por sus trabajos dedicados a la ufología. En su saga novelística Caballo de Troya relata un ficticio experimento de los Estados Unidos.
+Ha realizado trabajos para la televisión, conferencias, artículos de prensa y entrevistas con testigos de fenómenos ovni. Con frecuencia, estas obras han recibido críticas negativas por parte de diversos sectores, como es el caso de los escépticos</t>
+  </si>
+  <si>
+    <t>España</t>
+  </si>
+  <si>
+    <t>https://hips.hearstapps.com/hmg-prod.s3.amazonaws.com/images/jj-benitez-entrevista-esquire-1603726860.jpg</t>
+  </si>
+  <si>
+    <t>https://www.planetadelibros.com.mx/usuaris/autores/fotos/58/original/000057489_1_Bernal_Rafael_200_201509281925.jpg</t>
+  </si>
+  <si>
+    <t>Rafael Bernal y García Pimentel</t>
+  </si>
+  <si>
+    <t>Infarto</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/9/93/J._D._Salinger_%28Catcher_in_the_Rye_portrait%29.jpg</t>
+  </si>
+  <si>
+    <t>Jerome David Salinger (Nueva York, 1 de enero de 1919-Cornish, Nuevo Hampshire, 27 de enero de 2010)1​ fue un escritor estadounidense conocido principalmente por su novela El guardián entre el centeno (The Catcher in the Rye en inglés), que se convirtió en un clásico de la literatura moderna estadounidense casi desde el mismo momento de su publicación en 1951.</t>
+  </si>
+  <si>
+    <t>Rafael Bernal y García Pimentel (Ciudad de México, 28 de junio de 1915 - Berna, Suiza, 17 de septiembre de 1972) fue un diplomático, escritor, publicista, historiador y guionista mexicano, conocido ante todo por sus novelas policiacas, particularmente por El complot mongol.</t>
+  </si>
+  <si>
+    <t>Sylvia Plath (Pseudónimo: Victoria Lucas)</t>
+  </si>
+  <si>
+    <t>Sylvia Plath (Boston, 27 de octubre de 1932-Londres, 11 de febrero de 1963) fue una escritora y poeta estadounidense.4​ Considerada una de las cultivadoras del género de la poesía confesional,4​ sus obras más conocidas son sus poemarios El coloso y Ariel y su novela semiautobiográfica La campana de cristal, publicada bajo el seudónimo de «Victoria Lucas» cuatro meses antes de su suicidio.5​6​ Estuvo casada con el poeta Ted Hughes, quien tras su muerte se encargó de la edición de su poesía completa. En 1982 ganó un Premio Pulitzer póstumo por sus Poemas completos.4​
+Nacida en Boston, Massachusetts, Plath estudió en la Smith College de Massachusetts y, tras recibir una Beca Fullbright, en la Newnham College de Cambridge.4​ Tras casarse con Hughes en 1956, vivió junto a este en los Estados Unidos y luego en Inglaterra, donde tuvieron dos hijos antes de separarse en 1962.
+Plath, que estuvo clínicamente deprimida durante la mayor parte de su vida adulta y fue tratada varias veces con terapia electroconvulsiva (TEC),4​ se suicidó en 1963</t>
+  </si>
+  <si>
+    <t>Suicidio</t>
+  </si>
+  <si>
+    <t>https://cdn.zendalibros.com/wp-content/uploads/2018/01/sylvia-plath.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/61Hj3mQOahL._SX450_.jpg</t>
+  </si>
+  <si>
+    <t>Gayle Forman (Los Ángeles, 5 de junio de 1970) es una escritora americana de literatura juvenil, conocida por su novela Sí Decido Quedarme (If I Stay), la cual consiguió el best seller de literatura juvenil en The New York Times y fue llevada al cine en 2014.</t>
+  </si>
+  <si>
+    <t>Joanne Rowling1​ (Yate, 31 de julio de 1965), quien escribe bajo los seudónimos J. K. Rowling2​ y Robert Galbraith, es una escritora, productora de cine y guionista británica, conocida por ser la autora de la serie de libros Harry Potter, que han superado los quinientos millones de ejemplares vendidos.3​
+Este éxito literario supuso que la Sunday Times Rich List de 2008 estimase la fortuna de Rowling en 560 millones de libras, lo que la situó como la duodécima mujer más rica en el Reino Unido.4​ Asimismo, Forbes ubicó a Rowling en el cuadragésimo puesto en su lista de las celebridades más poderosas de 20075​ y la revista Time la seleccionó como «personaje del año» ese mismo año, resaltando la inspiración social, moral y política que les ha dado a los personajes de Harry Potter.6​
+Rowling es una conocida filántropa que apoya instituciones de caridad como Comic Relief, One Parent Families y Multiple Sclerosis Society of Great Britain.</t>
+  </si>
+  <si>
+    <t>Joanne Rowling (J.K Rowling)</t>
+  </si>
+  <si>
+    <t>https://cdn-3.expansion.mx/dims4/default/8f1fc42/2147483647/strip/true/crop/1000x1368+0+0/resize/1200x1642!/format/webp/quality/90/?url=https%3A%2F%2Fcdn-3.expansion.mx%2F0d%2F68%2F9897cac047dc80218fa427068f22%2Fgettyimages-1061365848.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/3/36/Philip_K_Dick_in_early_1960s_%28photo_by_Arthur_Knight%29_%28cropped%29.jpg/1200px-Philip_K_Dick_in_early_1960s_%28photo_by_Arthur_Knight%29_%28cropped%29.jpg</t>
+  </si>
+  <si>
+    <t>Derrame Cerebral</t>
+  </si>
+  <si>
+    <t>Philip Kindred Dick (Chicago, Illinois; 16 de diciembre de 1928-Santa Ana, California; 2 de marzo de 1982), más conocido como Philip K. Dick, fue un escritor y novelista estadounidense de ciencia ficción, que influyó notablemente en dicho género.
+Trató temas como la sociología, la política y la metafísica en sus primeras novelas, donde predominaban las empresas monopolísticas, los gobiernos autoritarios y los estados alterados de conciencia. En sus obras posteriores, el enfoque temático reflejó claramente su interés personal en la metafísica y la teología. A menudo se basó en su propia experiencia vital, y reflejó su obsesión con las drogas, la paranoia y la esquizofrenia en novelas como A Scanner Darkly y SIVAINVI.1​ La novela El hombre en el castillo, galardonada con el premio Hugo a la mejor novela en 1963,2​ está considerada como una obra maestra del subgénero de la ciencia ficción denominado «ucronía». Fluyan mis lágrimas, dijo el policía, una novela sobre una estrella televisiva que vive en un estado policial en un cercano futuro distópico, ganó el premio John W. Campbell Memorial a la mejor novela en 1975.</t>
+  </si>
+  <si>
+    <t>Desconocido</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/d/d8/JohnKennethTurner.jpg</t>
+  </si>
+  <si>
+    <t>John Kenneth Turner (1879-1948) fue un escritor y periodista nacido en Oregón, Estados Unidos.
+A los 17 años publicó su primer periódico titulado "Stockton Saturday Night" dedicado a denunciar políticos y empresarios corruptos. Turner fue estudiante de la Universidad de California y se casó con la profesora Ethel Duffy Turner. La pareja se estableció en San Francisco; pero el terremoto de 1906 los obligó a trasladarse a Portland y luego a Los Ángeles, donde Turner obtuvo un empleo como reportero del diario Los Angeles Express.</t>
+  </si>
+  <si>
+    <t>Juan Nepomuceno Carlos Pérez Rulfo Vizcaíno</t>
+  </si>
+  <si>
+    <t>México</t>
+  </si>
+  <si>
+    <t>Cáncer de Pulmón</t>
+  </si>
+  <si>
+    <t>https://www.elindependiente.com/wp-content/uploads/2017/05/juan-rulfo-caballero-bonald-1440x808.jpg</t>
+  </si>
+  <si>
+    <t>Juan Nepomuceno Carlos Pérez Rulfo Vizcaínonota 1​ (Apulco,3​4​ 16 de mayo de 1917-Ciudad de México, 7 de enero de 1986) fue un escritor, guionista y fotógrafo mexicano, perteneciente a la Generación del 52.5​6​ Es considerado uno de los escritores hispanoamericanos más importantes del siglo XX.7​8​ Su reputación se asienta en dos de sus tres obras narrativas: el libro de cuentos El Llano en llamas, publicado en 1953, y su novela Pedro Páramo, publicada en 1955.</t>
+  </si>
+  <si>
+    <t>Stephen Edwin King</t>
+  </si>
+  <si>
+    <t>https://www.latercera.com/resizer/NCXgvBGfnPbyZHK_0UyLT2VPiC0=/900x600/smart/cloudfront-us-east-1.images.arcpublishing.com/copesa/LAGOZGASXVGWPASNWYYP3IAPV4.jpg</t>
+  </si>
+  <si>
+    <t>Stephen Edwin King (pronunciación: /ˈstiːvən ˈɛdwɪn ˈkɪŋ/) (Portland, Maine; 21 de septiembre de 1947), más conocido como Stephen King y ocasionalmente por su pseudónimo Richard Bachman, es un escritor estadounidense de novelas de terror, ficción sobrenatural, misterio, ciencia ficción y literatura fantástica. Sus libros han vendido más de 350 millones de ejemplares1​ y en su mayoría han sido adaptados al cine y a la televisión. Ha publicado 61 novelas (siete de ellas, bajo el pseudónimo Richard Bachman) y siete libros de no ficción. Ha escrito, además, alrededor de doscientos relatos y novelas cortas, la mayoría de los cuales han sido recogidos en once colecciones</t>
+  </si>
+  <si>
+    <t>Reino Unido</t>
+  </si>
+  <si>
+    <t>AUTHOR_ID</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/b/bb/Conan_doyle.jpg</t>
+  </si>
+  <si>
+    <t>Arthur Ignatius Conan Doyle (Edimburgo, 22 de mayo de 1859-Crowborough, 7 de julio de 1930) fue un escritor y médico británico, creador del célebre detective de ficción Sherlock Holmes. Fue un autor prolífico cuya obra incluye relatos de ciencia ficción, novela histórica, teatro y poesía.</t>
+  </si>
+  <si>
+    <t>Irán</t>
+  </si>
+  <si>
+    <t>Marjane Satrapi (en persa, مرجان ساتراپی , tr. Maryán Satrapí; AFI mærˈʤɔːne sɔːtrɔːˈpiː) (Rasht, Irán, 1969) es una historietista (guionista y dibujante), pintora1​ y directora franco-iraní que trabaja para el mercado francófono.</t>
+  </si>
+  <si>
+    <t>https://c8.alamy.com/compes/pm5b76/pelicula-de-persepolis-de-marjane-satrapi-2007-sony-pictures-classics-archivo-de-referencia-30738481tha-solo-para-uso-editorial-todos-los-derechos-reservados-pm5b76.jpg</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,13 +453,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,24 +778,998 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B18DC47-EF92-3540-9929-CAC5BE64413E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="42.5" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2">
+        <v>485</v>
+      </c>
+      <c r="G2">
+        <v>1979</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>727</v>
+      </c>
+      <c r="G3">
+        <v>1984</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4">
+        <v>221</v>
+      </c>
+      <c r="G4">
+        <v>1969</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <v>206</v>
+      </c>
+      <c r="G5">
+        <v>1951</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6">
+        <v>269</v>
+      </c>
+      <c r="G6">
+        <v>1963</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7">
+        <v>211</v>
+      </c>
+      <c r="G7">
+        <v>2009</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8">
+        <v>269</v>
+      </c>
+      <c r="G8">
+        <v>1997</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9">
+        <v>320</v>
+      </c>
+      <c r="G9">
+        <v>1998</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10">
+        <v>384</v>
+      </c>
+      <c r="G10">
+        <v>1999</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11">
+        <v>672</v>
+      </c>
+      <c r="G11">
+        <v>2000</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12">
+        <v>928</v>
+      </c>
+      <c r="G12">
+        <v>2003</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <v>272</v>
+      </c>
+      <c r="G13">
+        <v>1962</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14">
+        <v>292</v>
+      </c>
+      <c r="G14">
+        <v>1909</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15">
+        <v>153</v>
+      </c>
+      <c r="G15">
+        <v>1953</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16">
+        <v>1215</v>
+      </c>
+      <c r="G16">
+        <v>1986</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17">
+        <v>589</v>
+      </c>
+      <c r="G17">
+        <v>1977</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18">
+        <v>295</v>
+      </c>
+      <c r="G18">
+        <v>1887</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19">
+        <v>140</v>
+      </c>
+      <c r="G19">
+        <v>1890</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20">
+        <v>243</v>
+      </c>
+      <c r="G20">
+        <v>1902</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21">
+        <v>366</v>
+      </c>
+      <c r="G21">
+        <v>2000</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H14" r:id="rId1" xr:uid="{0BB9F56A-8D0F-0145-BBDC-A4B667224D44}"/>
+    <hyperlink ref="H15" r:id="rId2" xr:uid="{F1F85D79-A518-284C-B830-A33EBAD01F9B}"/>
+    <hyperlink ref="H13" r:id="rId3" xr:uid="{CD774173-E458-C648-B33C-5BE1CD110DD3}"/>
+    <hyperlink ref="H21" r:id="rId4" xr:uid="{9BF2C83D-371C-E843-8B17-7CCA941478C3}"/>
+    <hyperlink ref="H20" r:id="rId5" xr:uid="{6B298D2A-CCFF-4F46-846E-F33CEB177105}"/>
+    <hyperlink ref="H19" r:id="rId6" xr:uid="{E3DFA016-8261-F642-B257-AE66CD204160}"/>
+    <hyperlink ref="H17" r:id="rId7" xr:uid="{6979905C-97A5-2C47-88FC-306D35750171}"/>
+    <hyperlink ref="H16" r:id="rId8" xr:uid="{AA28190E-97D6-2D45-AECD-2CD95BE79CEE}"/>
+    <hyperlink ref="H8" r:id="rId9" xr:uid="{3C498386-50F4-9843-9866-36CE5475CF6E}"/>
+    <hyperlink ref="H9" r:id="rId10" xr:uid="{0575162A-C52A-684E-8EC1-D381C655081E}"/>
+    <hyperlink ref="H10" r:id="rId11" xr:uid="{0F2633D8-669F-2841-97D8-F68CCA152216}"/>
+    <hyperlink ref="H11" r:id="rId12" xr:uid="{C4AEFFE5-3EE6-C844-A0B1-7969D605C087}"/>
+    <hyperlink ref="H12" r:id="rId13" xr:uid="{DD06005E-7399-4A40-BF1B-9A5377C0E2FF}"/>
+    <hyperlink ref="H18" r:id="rId14" xr:uid="{0270A2F9-306A-2646-9E30-FD69C0B789D6}"/>
+    <hyperlink ref="H2" r:id="rId15" xr:uid="{3828E174-71CC-DA4D-9B84-8EF2CF31D491}"/>
+    <hyperlink ref="H3" r:id="rId16" xr:uid="{9FC9FF51-0364-DA4F-95B0-2D95414678D3}"/>
+    <hyperlink ref="H4" r:id="rId17" xr:uid="{D648CE6D-50C1-F740-9BE7-3B284D815BBD}"/>
+    <hyperlink ref="H5" r:id="rId18" xr:uid="{CAF115CC-16D1-0B42-9836-58886C94CB1C}"/>
+    <hyperlink ref="H6" r:id="rId19" xr:uid="{020CB093-BBA9-574C-B3E8-B32C313CDFA6}"/>
+    <hyperlink ref="H7" r:id="rId20" xr:uid="{77D695B5-1C39-3641-8120-9834B71D35DB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623A6429-10B5-204C-9C42-A3E9BB97694B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="40.5" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="388" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>1923</v>
+      </c>
+      <c r="D2">
+        <v>1986</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>1946</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4">
+        <v>1915</v>
+      </c>
+      <c r="D4">
+        <v>1972</v>
+      </c>
+      <c r="E4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>1919</v>
+      </c>
+      <c r="D5">
+        <v>2010</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6">
+        <v>1932</v>
+      </c>
+      <c r="D6">
+        <v>1963</v>
+      </c>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="153" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>1970</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8">
+        <v>1965</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>1928</v>
+      </c>
+      <c r="D9">
+        <v>1982</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="340" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>1879</v>
+      </c>
+      <c r="D10">
+        <v>1948</v>
+      </c>
+      <c r="E10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11">
+        <v>1917</v>
+      </c>
+      <c r="D11">
+        <v>1986</v>
+      </c>
+      <c r="E11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="404" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12">
+        <v>1947</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>1859</v>
+      </c>
+      <c r="D13">
+        <v>1930</v>
+      </c>
+      <c r="E13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>1969</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{A318BBB7-8967-D146-8030-FDF753A5B700}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{292077F5-F1FC-BF48-8B51-321CA687CB90}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{27D4EEE6-4F9B-D742-B391-EE6635337C10}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{DAA8B356-C844-114D-8466-3F8A22E33EA8}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{1E70A27E-07B5-1940-AAF1-9510342ECBF5}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{25BCB727-E638-9648-9E4C-14C04F89FC92}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{2963D377-D042-744E-B462-4CE01A705A91}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{959EBF19-AD98-124B-BF42-95059CF78AED}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{22D6D18C-CB00-0D42-8680-2D5A20161BB9}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{0A411740-FE30-4749-A70F-26BE06223099}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{CCDD16E9-429C-FE44-BCBB-A707655F3191}"/>
+    <hyperlink ref="G13" r:id="rId12" xr:uid="{B6014748-CB05-5449-AD3A-72D19BB604DC}"/>
+    <hyperlink ref="G14" r:id="rId13" xr:uid="{2EDF9567-CC6E-304F-8B97-7D4744EBEF70}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>